<commit_message>
probando si carga deuda privada
</commit_message>
<xml_diff>
--- a/DeudaPrivadaOrigen.xlsx
+++ b/DeudaPrivadaOrigen.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11370" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11370" uniqueCount="89">
   <si>
     <t>SectorINECorto</t>
   </si>
@@ -291,13 +291,16 @@
   <si>
     <t>bk</t>
   </si>
+  <si>
+    <t>Acreedor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -346,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -631,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5461" workbookViewId="0">
-      <selection activeCell="N5480" sqref="N5480"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +651,7 @@
         <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
dibuja el total de deuda privada pero no los sectores
</commit_message>
<xml_diff>
--- a/DeudaPrivadaOrigen.xlsx
+++ b/DeudaPrivadaOrigen.xlsx
@@ -16,6 +16,9 @@
     <sheet name="pivot" sheetId="2" r:id="rId2"/>
     <sheet name="datos y ponderadores" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DeudaPrivada!$A$1:$D$5581</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -635,7 +638,7 @@
   <dimension ref="A1:D5581"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>